<commit_message>
INX H, INX D
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfrosch/cs467/cs467-capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A661F0-762A-D047-97DB-C1E0EF9F6D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA18F1A-1A61-A244-8BD8-133FAE74C5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="780" windowWidth="11300" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2657,7 +2657,7 @@
   <dimension ref="A1:F257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7813,7 +7813,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A258:F259 A1:E1 A2:E2 A3:D3 A4:D4 A5:E5 A6:C6 A7:E7 A8:E8 A9:E9 A10:E10 A11:E11 A12:E12 A13:E13 A14:E14 A15:E15 A16:E16 A17:E17 A18:E18 A19:E19 A20:E20 A21:E21 A22:E22 A23:E23 A24:E24 A25:E25 A26:E26 A27:E27 A28:E28 A29:E29 A30:E30 A31:E31 A32:E32 A33:E33 A34:E34 A35:E35 A36:E36 A37:E37 A38:E38 A39:C39 A40:E40 A41:E41 A42:E42 A43:E43 A44:E44 A45:E45 A46:C46 A47:E47 A48:E48 A49:E49 A50:E50 A51:E51 A52:E52 A53:E53 A54:E54 A55:E55 A56:E56 A57:E57 A58:E58 A59:E59 A60:E60 A61:E61 A62:E62 A63:E63 A64:E64 A65:E65 A66:E66 A67:E67 A68:E68 A69:E69 A70:E70 A71:E71 A72:E72 A73:E73 A74:E74 A75:E75 A76:E76 A77:E77 A78:E78 A79:E79 A80:E80 A81:E81 A82:E82 A83:E83 A84:E84 A85:E85 A86:E86 A87:E87 A88:E88 A89:E89 A90:E90 A91:E91 A92:E92 A93:E93 A94:E94 A95:E95 A96:E96 A97:E97 A98:E98 A99:E99 A100:E100 A101:E101 A102:E102 A103:E103 A104:E104 A105:E105 A106:E106 A107:E107 A108:E108 A109:E109 A110:E110 A111:E111 A112:E112 A113:E113 A114:E114 A115:E115 A116:E116 A117:E117 A118:E118 A119:E119 A120:E120 A121:E121 A122:E122 A123:E123 A124:E124 A125:E125 A126:E126 A127:E127 A128:E128 A129:E129 A130:E130 A131:E131 A132:E132 A133:E133 A134:E134 A135:E135 A136:E136 A137:E137 A138:E138 A139:E139 A140:E140 A141:E141 A142:E142 A143:E143 A144:E144 A145:E145 A146:E146 A147:E147 A148:E148 A149:E149 A150:E150 A151:E151 A152:E152 A153:E153 A154:E154 A155:E155 A156:E156 A157:E157 A158:E158 A159:E159 A160:E160 A161:E161 A162:E162 A163:E163 A164:E164 A165:E165 A166:E166 A167:E167 A168:E168 A169:E169 A170:E170 A171:E171 A172:E172 A173:E173 A174:E174 A175:E175 A176:E176 A177:E177 A178:E178 A179:E179 A180:E180 A181:E181 A182:E182 A183:E183 A184:E184 A185:E185 A186:E186 A187:E187 A188:E188 A189:E189 A190:E190 A191:E191 A192:E192 A193:E193 A194:E194 A195:E195 A196:E196 A197:E197 A198:E198 A199:E199 A200:E200 A201:E201 A202:E202 A203:E203 A204:E204 A205:E205 A206:E206 A207:E207 A208:E208 A209:E209 A210:E210 A211:E211 A212:E212 A213:E213 A214:E214 A215:E215 A216:E216 A217:E217 A218:E218 A219:E219 A220:E220 A221:E221 A222:E222 A223:E223 A224:E224 A225:E225 A226:E226 A227:E227 A228:E228 A229:E229 A230:E230 A231:E231 A232:E232 A233:E233 A234:E234 A235:E235 A236:E236 A237:E237 A238:E238 A239:E239 A240:E240 A241:E241 A242:E242 A243:E243 A244:E244 A245:E245 A246:E246 A247:E247 A248:E248 A249:E249 A250:E250 A251:E251 A252:E252 A253:E253 A254:E254 A255:E255 A256:E256 A257:E257 E6 E39 E46" numberStoredAsText="1"/>
+    <ignoredError sqref="A258:F259 A1:E1 A2:E2 A3:D3 A4:D4 A5:E5 A6:C6 A7:E7 A8:E8 A9:E9 A10:E10 A11:E11 A12:E12 A13:E13 A14:E14 A15:E15 A16:E16 A17:E17 A18:E18 A19:D19 A20:E20 A21:E21 A22:E22 A23:E23 A24:E24 A25:E25 A26:E26 A27:E27 A28:D28 A29:E29 A30:E30 A31:E31 A32:E32 A33:E33 A34:E34 A35:E35 A36:E36 A37:E37 A38:E38 A39:C39 A40:E40 A41:E41 A42:E42 A43:E43 A44:E44 A45:E45 A46:C46 A47:E47 A48:E48 A49:E49 A50:E50 A51:E51 A52:E52 A53:E53 A54:E54 A55:E55 A56:E56 A57:E57 A58:E58 A59:E59 A60:E60 A61:E61 A62:E62 A63:E63 A64:E64 A65:E65 A66:E66 A67:E67 A68:E68 A69:E69 A70:E70 A71:E71 A72:E72 A73:E73 A74:E74 A75:E75 A76:E76 A77:E77 A78:E78 A79:E79 A80:E80 A81:E81 A82:E82 A83:E83 A84:E84 A85:E85 A86:E86 A87:E87 A88:E88 A89:E89 A90:E90 A91:E91 A92:E92 A93:E93 A94:E94 A95:E95 A96:E96 A97:E97 A98:E98 A99:E99 A100:E100 A101:E101 A102:E102 A103:E103 A104:E104 A105:E105 A106:E106 A107:E107 A108:E108 A109:E109 A110:E110 A111:E111 A112:E112 A113:E113 A114:E114 A115:E115 A116:E116 A117:E117 A118:E118 A119:E119 A120:E120 A121:E121 A122:E122 A123:E123 A124:E124 A125:E125 A126:E126 A127:E127 A128:E128 A129:E129 A130:E130 A131:E131 A132:E132 A133:E133 A134:E134 A135:E135 A136:E136 A137:E137 A138:E138 A139:E139 A140:E140 A141:E141 A142:E142 A143:E143 A144:E144 A145:E145 A146:E146 A147:E147 A148:E148 A149:E149 A150:E150 A151:E151 A152:E152 A153:E153 A154:E154 A155:E155 A156:E156 A157:E157 A158:E158 A159:E159 A160:E160 A161:E161 A162:E162 A163:E163 A164:E164 A165:E165 A166:E166 A167:E167 A168:E168 A169:E169 A170:E170 A171:E171 A172:E172 A173:E173 A174:E174 A175:E175 A176:E176 A177:E177 A178:E178 A179:E179 A180:E180 A181:E181 A182:E182 A183:E183 A184:E184 A185:E185 A186:E186 A187:E187 A188:E188 A189:E189 A190:E190 A191:E191 A192:E192 A193:E193 A194:E194 A195:E195 A196:E196 A197:E197 A198:E198 A199:E199 A200:E200 A201:E201 A202:E202 A203:E203 A204:E204 A205:E205 A206:E206 A207:E207 A208:E208 A209:E209 A210:E210 A211:E211 A212:E212 A213:E213 A214:E214 A215:E215 A216:E216 A217:E217 A218:E218 A219:E219 A220:E220 A221:E221 A222:E222 A223:E223 A224:E224 A225:E225 A226:E226 A227:E227 A228:E228 A229:E229 A230:E230 A231:E231 A232:E232 A233:E233 A234:E234 A235:E235 A236:E236 A237:E237 A238:E238 A239:E239 A240:E240 A241:E241 A242:E242 A243:E243 A244:E244 A245:E245 A246:E246 A247:E247 A248:E248 A249:E249 A250:E250 A251:E251 A252:E252 A253:E253 A254:E254 A255:E255 A256:E256 A257:E257 E6 E39 E46" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>